<commit_message>
full refactoring and new GAM analysis
</commit_message>
<xml_diff>
--- a/data/flu.xlsx
+++ b/data/flu.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trenthenderson/Documents/Git/influenza-impact/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nousgroup-my.sharepoint.com/personal/trent_henderson_nousgroup_com_au/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFC43F62-E2BB-AB4C-A49B-10D5B3C61C7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BD4BD394-5D3B-4F47-9D6F-7F80BE81FFF2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="460" windowWidth="28800" windowHeight="16800" xr2:uid="{1B601E99-FB95-4285-9F1D-17A41476DCD5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{E3E66798-3CA3-46A8-B23A-264369CFD953}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,11 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -70,26 +75,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF222222"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF222222"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -112,10 +104,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,877 +419,1153 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F71F9BDE-F86A-4112-A87D-980D528F4522}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10B50109-8A64-4312-94D4-6CC7CB9F41B0}">
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>2001</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2">
         <v>0.1</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2">
         <v>0.1</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2">
         <v>0.1</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2">
         <v>0</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2">
         <v>0.1</v>
       </c>
-      <c r="G2" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="H2" s="2">
+      <c r="G2">
+        <v>0.2</v>
+      </c>
+      <c r="H2">
         <v>1</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2">
         <v>2.5</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2">
         <v>1.7</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2">
         <v>0.6</v>
       </c>
-      <c r="L2" s="2">
+      <c r="L2">
         <v>0.3</v>
       </c>
-      <c r="M2" s="2">
+      <c r="M2">
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>2002</v>
       </c>
-      <c r="B3" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="F3" s="2">
+      <c r="B3">
+        <v>0.2</v>
+      </c>
+      <c r="C3">
+        <v>0.2</v>
+      </c>
+      <c r="D3">
+        <v>0.2</v>
+      </c>
+      <c r="E3">
+        <v>0.2</v>
+      </c>
+      <c r="F3">
         <v>0.8</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3">
         <v>2.7</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3">
         <v>5.0999999999999996</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3">
         <v>6</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3">
         <v>2.2000000000000002</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3">
         <v>0.7</v>
       </c>
-      <c r="L3" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="M3" s="2">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
+      <c r="L3">
+        <v>0.2</v>
+      </c>
+      <c r="M3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>2003</v>
       </c>
-      <c r="B4" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="C4" s="2">
+      <c r="B4">
+        <v>0.2</v>
+      </c>
+      <c r="C4">
         <v>0.1</v>
       </c>
-      <c r="D4" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="E4" s="2">
+      <c r="D4">
+        <v>0.2</v>
+      </c>
+      <c r="E4">
         <v>0.3</v>
       </c>
-      <c r="F4" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="G4" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="H4" s="2">
+      <c r="F4">
+        <v>0.2</v>
+      </c>
+      <c r="G4">
+        <v>0.2</v>
+      </c>
+      <c r="H4">
         <v>1</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4">
         <v>7.8</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4">
         <v>6.5</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4">
         <v>0.9</v>
       </c>
-      <c r="L4" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="M4" s="2">
+      <c r="L4">
+        <v>0.2</v>
+      </c>
+      <c r="M4">
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>2004</v>
       </c>
-      <c r="B5" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="D5" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="G5" s="2">
+      <c r="B5">
+        <v>0.2</v>
+      </c>
+      <c r="C5">
+        <v>0.2</v>
+      </c>
+      <c r="D5">
+        <v>0.2</v>
+      </c>
+      <c r="E5">
+        <v>0.2</v>
+      </c>
+      <c r="F5">
+        <v>0.2</v>
+      </c>
+      <c r="G5">
         <v>0.4</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5">
         <v>0.5</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5">
         <v>1.3</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5">
         <v>3.6</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5">
         <v>2.1</v>
       </c>
-      <c r="L5" s="2">
+      <c r="L5">
         <v>1</v>
       </c>
-      <c r="M5" s="2">
+      <c r="M5">
         <v>0.6</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>2005</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6">
         <v>0.7</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6">
         <v>0.6</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6">
         <v>0.4</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6">
         <v>0.6</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6">
         <v>0.7</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6">
         <v>2.5</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6">
         <v>5.0999999999999996</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6">
         <v>6.7</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6">
         <v>3.2</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6">
         <v>1.2</v>
       </c>
-      <c r="L6" s="2">
+      <c r="L6">
         <v>0.5</v>
       </c>
-      <c r="M6" s="2">
+      <c r="M6">
         <v>0.3</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>2006</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7">
         <v>0.3</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7">
         <v>0.3</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7">
         <v>0.4</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7">
         <v>0.3</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7">
         <v>0.5</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7">
         <v>1.1000000000000001</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7">
         <v>2.7</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7">
         <v>5.3</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J7">
         <v>3.2</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7">
         <v>1</v>
       </c>
-      <c r="L7" s="2">
+      <c r="L7">
         <v>0.7</v>
       </c>
-      <c r="M7" s="2">
+      <c r="M7">
         <v>0.4</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>2007</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8">
         <v>0.5</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8">
         <v>0.5</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8">
         <v>0.6</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8">
         <v>0.6</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8">
         <v>0.6</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8">
         <v>1.6</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8">
         <v>12.1</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8">
         <v>24.7</v>
       </c>
-      <c r="J8" s="2">
+      <c r="J8">
         <v>5.9</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K8">
         <v>2</v>
       </c>
-      <c r="L8" s="2">
+      <c r="L8">
         <v>0.8</v>
       </c>
-      <c r="M8" s="2">
+      <c r="M8">
         <v>0.6</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>2008</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9">
         <v>0.5</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9">
         <v>0.7</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9">
         <v>0.8</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9">
         <v>0.9</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9">
         <v>1.2</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9">
         <v>1.3</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9">
         <v>3.1</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9">
         <v>12.3</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J9">
         <v>15</v>
       </c>
-      <c r="K9" s="2">
+      <c r="K9">
         <v>4.8</v>
       </c>
-      <c r="L9" s="2">
+      <c r="L9">
         <v>1.6</v>
       </c>
-      <c r="M9" s="2">
+      <c r="M9">
         <v>0.9</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>2009</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10">
         <v>0.8</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10">
         <v>0.6</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10">
         <v>0.8</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10">
         <v>1.3</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10">
         <v>11.8</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10">
         <v>56.8</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10">
         <v>137.6</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I10">
         <v>51.3</v>
       </c>
-      <c r="J10" s="2">
+      <c r="J10">
         <v>7.5</v>
       </c>
-      <c r="K10" s="2">
+      <c r="K10">
         <v>1.9</v>
       </c>
-      <c r="L10" s="2">
+      <c r="L10">
         <v>1.2</v>
       </c>
-      <c r="M10" s="2">
+      <c r="M10">
         <v>0.8</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>2010</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11">
         <v>0.7</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11">
         <v>0.6</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11">
         <v>0.8</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11">
         <v>1.2</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11">
         <v>1</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11">
         <v>1.4</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11">
         <v>3.4</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11">
         <v>11.1</v>
       </c>
-      <c r="J11" s="2">
+      <c r="J11">
         <v>22.6</v>
       </c>
-      <c r="K11" s="2">
+      <c r="K11">
         <v>9.8000000000000007</v>
       </c>
-      <c r="L11" s="2">
+      <c r="L11">
         <v>4.3</v>
       </c>
-      <c r="M11" s="2">
+      <c r="M11">
         <v>4.3</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>2011</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12">
         <v>4</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12">
         <v>3.8</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12">
         <v>4.0999999999999996</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12">
         <v>3</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12">
         <v>4</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12">
         <v>11.6</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12">
         <v>25.3</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12">
         <v>34.4</v>
       </c>
-      <c r="J12" s="2">
+      <c r="J12">
         <v>18.600000000000001</v>
       </c>
-      <c r="K12" s="2">
+      <c r="K12">
         <v>7.7</v>
       </c>
-      <c r="L12" s="2">
+      <c r="L12">
         <v>3.4</v>
       </c>
-      <c r="M12" s="2">
+      <c r="M12">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>2012</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13">
         <v>1.4</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13">
         <v>1.6</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13">
         <v>2.7</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13">
         <v>2.5</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13">
         <v>5.0999999999999996</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13">
         <v>24.5</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13">
         <v>61.3</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13">
         <v>62.8</v>
       </c>
-      <c r="J13" s="2">
+      <c r="J13">
         <v>20.7</v>
       </c>
-      <c r="K13" s="2">
+      <c r="K13">
         <v>6.2</v>
       </c>
-      <c r="L13" s="2">
+      <c r="L13">
         <v>4.5</v>
       </c>
-      <c r="M13" s="2">
+      <c r="M13">
         <v>2.9</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>2013</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14">
         <v>3.1</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14">
         <v>3.2</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14">
         <v>3.7</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14">
         <v>2.7</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14">
         <v>3.4</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14">
         <v>4.7</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H14">
         <v>12.6</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I14">
         <v>33.299999999999997</v>
       </c>
-      <c r="J14" s="2">
+      <c r="J14">
         <v>27.8</v>
       </c>
-      <c r="K14" s="2">
+      <c r="K14">
         <v>12.8</v>
       </c>
-      <c r="L14" s="2">
+      <c r="L14">
         <v>8.6</v>
       </c>
-      <c r="M14" s="2">
+      <c r="M14">
         <v>6.5</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>2014</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15">
         <v>6</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15">
         <v>4.9000000000000004</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15">
         <v>5.3</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15">
         <v>4.5</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15">
         <v>5.6</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15">
         <v>9.4</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15">
         <v>42.3</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I15">
         <v>114.2</v>
       </c>
-      <c r="J15" s="2">
+      <c r="J15">
         <v>69.400000000000006</v>
       </c>
-      <c r="K15" s="2">
+      <c r="K15">
         <v>16.3</v>
       </c>
-      <c r="L15" s="2">
+      <c r="L15">
         <v>5.6</v>
       </c>
-      <c r="M15" s="2">
+      <c r="M15">
         <v>4.8</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>2015</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16">
         <v>5.2</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16">
         <v>5.6</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16">
         <v>8.3000000000000007</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16">
         <v>9.3000000000000007</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16">
         <v>10.6</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16">
         <v>21.1</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16">
         <v>55.8</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I16">
         <v>164.6</v>
       </c>
-      <c r="J16" s="2">
+      <c r="J16">
         <v>113.7</v>
       </c>
-      <c r="K16" s="2">
+      <c r="K16">
         <v>19.899999999999999</v>
       </c>
-      <c r="L16" s="2">
+      <c r="L16">
         <v>5</v>
       </c>
-      <c r="M16" s="2">
+      <c r="M16">
         <v>3.3</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>2016</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17">
         <v>4.8</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17">
         <v>8.1</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17">
         <v>11</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17">
         <v>10.1</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17">
         <v>8.5</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17">
         <v>11.7</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17">
         <v>37.4</v>
       </c>
-      <c r="I17" s="2">
+      <c r="I17">
         <v>121.7</v>
       </c>
-      <c r="J17" s="2">
+      <c r="J17">
         <v>100.1</v>
       </c>
-      <c r="K17" s="2">
+      <c r="K17">
         <v>35</v>
       </c>
-      <c r="L17" s="2">
+      <c r="L17">
         <v>16.7</v>
       </c>
-      <c r="M17" s="2">
+      <c r="M17">
         <v>10.6</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>2017</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18">
         <v>11.2</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18">
         <v>11.2</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18">
         <v>11.5</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18">
         <v>7.9</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18">
         <v>13.4</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G18">
         <v>31.7</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H18">
         <v>135.69999999999999</v>
       </c>
-      <c r="I18" s="2">
+      <c r="I18">
         <v>404.3</v>
       </c>
-      <c r="J18" s="2">
+      <c r="J18">
         <v>308.39999999999998</v>
       </c>
-      <c r="K18" s="2">
+      <c r="K18">
         <v>64.3</v>
       </c>
-      <c r="L18" s="2">
+      <c r="L18">
         <v>13.7</v>
       </c>
-      <c r="M18" s="2">
+      <c r="M18">
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>2018</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19">
         <v>15</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19">
         <v>13.9</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19">
         <v>12.7</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19">
         <v>7.9</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19">
         <v>6.9</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G19">
         <v>8</v>
       </c>
-      <c r="H19" s="2">
+      <c r="H19">
         <v>15.9</v>
       </c>
-      <c r="I19" s="2">
+      <c r="I19">
         <v>32.700000000000003</v>
       </c>
-      <c r="J19" s="2">
+      <c r="J19">
         <v>46.1</v>
       </c>
-      <c r="K19" s="2">
+      <c r="K19">
         <v>29.3</v>
       </c>
-      <c r="L19" s="2">
+      <c r="L19">
         <v>22.2</v>
       </c>
-      <c r="M19" s="2">
+      <c r="M19">
         <v>25.1</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20">
         <v>2019</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20">
         <v>26.9</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20">
         <v>28.3</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20">
         <v>44.3</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20">
         <v>73.7</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20">
         <v>120.9</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20">
         <v>228.5</v>
       </c>
-      <c r="H20" s="2">
+      <c r="H20">
         <v>276.39999999999998</v>
       </c>
-      <c r="I20" s="2">
+      <c r="I20">
         <v>240.9</v>
       </c>
-      <c r="J20" s="2">
+      <c r="J20">
         <v>132.19999999999999</v>
       </c>
-      <c r="K20" s="2">
+      <c r="K20">
         <v>32.6</v>
       </c>
-      <c r="L20" s="2">
+      <c r="L20">
         <v>14.7</v>
       </c>
-      <c r="M20" s="2">
+      <c r="M20">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21">
         <v>2020</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21">
         <v>27.5</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21">
         <v>28.3</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21">
         <v>23.3</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21">
         <v>1.2</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21">
         <v>0.9</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G21">
         <v>0.9</v>
       </c>
-      <c r="H21" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="I21" s="2">
+      <c r="H21">
+        <v>0.7</v>
+      </c>
+      <c r="I21">
         <v>0.5</v>
       </c>
-      <c r="J21" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="K21" s="2">
+      <c r="J21">
+        <v>0.2</v>
+      </c>
+      <c r="K21">
         <v>0.1</v>
       </c>
-      <c r="L21" s="2">
-        <v>0</v>
-      </c>
-      <c r="M21" s="2">
-        <v>0</v>
+      <c r="L21">
+        <v>0.2</v>
+      </c>
+      <c r="M21">
+        <v>0.3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000D983E4C275FFA43AE3CF7F85B8DCFFE" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ff55a39190ac39bc273e7da1329f9340">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b3209b40-1402-47c1-b5a6-58dc853098dc" xmlns:ns4="2ebe818b-62b6-47e6-a828-50fa4c3920bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="49a92aa9779c4c1e90175f8403d27ad0" ns3:_="" ns4:_="">
+    <xsd:import namespace="b3209b40-1402-47c1-b5a6-58dc853098dc"/>
+    <xsd:import namespace="2ebe818b-62b6-47e6-a828-50fa4c3920bf"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns4:SharingHintHash" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceKeyPoints" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="b3209b40-1402-47c1-b5a6-58dc853098dc" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="13" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="14" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="15" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="16" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="17" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="18" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="19" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="2ebe818b-62b6-47e6-a828-50fa4c3920bf" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="10" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="11" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="SharingHintHash" ma:index="12" nillable="true" ma:displayName="Sharing Hint Hash" ma:hidden="true" ma:internalName="SharingHintHash" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF311E7B-BD09-4166-BB04-2BFC401DEFDE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b3209b40-1402-47c1-b5a6-58dc853098dc"/>
+    <ds:schemaRef ds:uri="2ebe818b-62b6-47e6-a828-50fa4c3920bf"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD842F24-7650-4945-9D8D-C27034CB153A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75580783-1F7B-4F21-9AE8-2274B43B7A75}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2ebe818b-62b6-47e6-a828-50fa4c3920bf"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="b3209b40-1402-47c1-b5a6-58dc853098dc"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>